<commit_message>
valid now with older version
</commit_message>
<xml_diff>
--- a/Files/Templates/createfilesfromxpath_A.xlsx
+++ b/Files/Templates/createfilesfromxpath_A.xlsx
@@ -15,7 +15,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">A1ToA4_mandatorychecks!$A$1:$N$65</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">bizrule!$A$1:$Q$80</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3083" uniqueCount="1227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3006" uniqueCount="1228">
   <si>
     <t>y</t>
   </si>
@@ -4363,6 +4363,9 @@
   </si>
   <si>
     <t>TC80_B25_offLabel_197_bizrul_NA251true_err</t>
+  </si>
+  <si>
+    <t>XPATH</t>
   </si>
 </sst>
 </file>
@@ -4512,7 +4515,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4692,9 +4695,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -4763,7 +4763,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9F749E25-1DAB-404D-BCE5-F308C06BEBE2}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F749E25-1DAB-404D-BCE5-F308C06BEBE2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4807,7 +4807,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{92C5092D-9FA9-4251-A659-0E7C51D8FDA3}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92C5092D-9FA9-4251-A659-0E7C51D8FDA3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4851,7 +4851,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{91728589-A071-42C5-9AEB-70633789F200}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91728589-A071-42C5-9AEB-70633789F200}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4895,7 +4895,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FABB97FF-63EE-4982-9CBB-205A4CE1974A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FABB97FF-63EE-4982-9CBB-205A4CE1974A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5179,7 +5179,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5190,9 +5190,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:W80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L23" sqref="L23"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="9.75" customHeight="1"/>
@@ -5206,7 +5206,7 @@
     <col min="7" max="7" width="17.33203125" style="59" customWidth="1"/>
     <col min="8" max="8" width="9.109375" style="59" collapsed="1"/>
     <col min="9" max="9" width="17.5546875" style="59" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="8" style="69" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="8" style="68" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="39.5546875" style="64" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="33.44140625" style="64" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="42.88671875" style="65" customWidth="1" collapsed="1"/>
@@ -5247,8 +5247,8 @@
       <c r="I1" s="50" t="s">
         <v>1020</v>
       </c>
-      <c r="J1" s="67" t="s">
-        <v>29</v>
+      <c r="J1" s="50" t="s">
+        <v>1227</v>
       </c>
       <c r="K1" s="50" t="s">
         <v>30</v>
@@ -5300,20 +5300,19 @@
       <c r="I2" s="54" t="s">
         <v>348</v>
       </c>
-      <c r="J2" s="68" t="s">
+      <c r="J2" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="K2" s="55" t="str">
-        <f>CONCATENATE(B2,"_",C2,"_",D2,"_",E2,"_",F2,"_",G2,"_",H2)</f>
-        <v>TC1_A312_LastName_39_mand_validtext_P</v>
+      <c r="K2" s="55" t="s">
+        <v>1148</v>
       </c>
       <c r="L2" s="55" t="s">
         <v>1148</v>
       </c>
-      <c r="M2" s="75" t="s">
+      <c r="M2" s="74" t="s">
         <v>979</v>
       </c>
-      <c r="N2" s="75" t="s">
+      <c r="N2" s="74" t="s">
         <v>947</v>
       </c>
       <c r="O2" s="61" t="s">
@@ -5327,9 +5326,7 @@
       </c>
     </row>
     <row r="3" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A3" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A3" s="54"/>
       <c r="B3" s="54" t="s">
         <v>1060</v>
       </c>
@@ -5354,7 +5351,7 @@
       <c r="I3" s="54" t="s">
         <v>349</v>
       </c>
-      <c r="J3" s="68" t="s">
+      <c r="J3" s="67" t="s">
         <v>47</v>
       </c>
       <c r="K3" s="55" t="str">
@@ -5364,10 +5361,10 @@
       <c r="L3" s="55" t="s">
         <v>1149</v>
       </c>
-      <c r="M3" s="75" t="s">
+      <c r="M3" s="74" t="s">
         <v>980</v>
       </c>
-      <c r="N3" s="75" t="s">
+      <c r="N3" s="74" t="s">
         <v>948</v>
       </c>
       <c r="O3" s="61" t="s">
@@ -5381,9 +5378,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A4" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A4" s="54"/>
       <c r="B4" s="54" t="s">
         <v>1061</v>
       </c>
@@ -5408,7 +5403,7 @@
       <c r="I4" s="54" t="s">
         <v>351</v>
       </c>
-      <c r="J4" s="68" t="s">
+      <c r="J4" s="67" t="s">
         <v>50</v>
       </c>
       <c r="K4" s="55" t="str">
@@ -5418,10 +5413,10 @@
       <c r="L4" s="55" t="s">
         <v>1150</v>
       </c>
-      <c r="M4" s="75" t="s">
+      <c r="M4" s="74" t="s">
         <v>981</v>
       </c>
-      <c r="N4" s="75" t="s">
+      <c r="N4" s="74" t="s">
         <v>949</v>
       </c>
       <c r="O4" s="61" t="s">
@@ -5435,9 +5430,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A5" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A5" s="54"/>
       <c r="B5" s="54" t="s">
         <v>1062</v>
       </c>
@@ -5462,7 +5455,7 @@
       <c r="I5" s="54" t="s">
         <v>350</v>
       </c>
-      <c r="J5" s="68" t="s">
+      <c r="J5" s="67" t="s">
         <v>48</v>
       </c>
       <c r="K5" s="55" t="str">
@@ -5472,10 +5465,10 @@
       <c r="L5" s="55" t="s">
         <v>1151</v>
       </c>
-      <c r="M5" s="75" t="s">
+      <c r="M5" s="74" t="s">
         <v>331</v>
       </c>
-      <c r="N5" s="75"/>
+      <c r="N5" s="74"/>
       <c r="O5" s="61" t="s">
         <v>359</v>
       </c>
@@ -5487,9 +5480,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A6" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A6" s="54"/>
       <c r="B6" s="54" t="s">
         <v>1063</v>
       </c>
@@ -5514,7 +5505,7 @@
       <c r="I6" s="54" t="s">
         <v>347</v>
       </c>
-      <c r="J6" s="68" t="s">
+      <c r="J6" s="67" t="s">
         <v>319</v>
       </c>
       <c r="K6" s="55" t="str">
@@ -5524,10 +5515,10 @@
       <c r="L6" s="55" t="s">
         <v>1152</v>
       </c>
-      <c r="M6" s="75" t="s">
+      <c r="M6" s="74" t="s">
         <v>331</v>
       </c>
-      <c r="N6" s="75"/>
+      <c r="N6" s="74"/>
       <c r="O6" s="61" t="s">
         <v>359</v>
       </c>
@@ -5539,9 +5530,7 @@
       </c>
     </row>
     <row r="7" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A7" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A7" s="54"/>
       <c r="B7" s="54" t="s">
         <v>1064</v>
       </c>
@@ -5566,7 +5555,7 @@
       <c r="I7" s="54" t="s">
         <v>346</v>
       </c>
-      <c r="J7" s="68" t="s">
+      <c r="J7" s="67" t="s">
         <v>326</v>
       </c>
       <c r="K7" s="55" t="str">
@@ -5576,8 +5565,8 @@
       <c r="L7" s="55" t="s">
         <v>1153</v>
       </c>
-      <c r="M7" s="75"/>
-      <c r="N7" s="75"/>
+      <c r="M7" s="74"/>
+      <c r="N7" s="74"/>
       <c r="O7" s="61" t="s">
         <v>355</v>
       </c>
@@ -5589,9 +5578,7 @@
       </c>
     </row>
     <row r="8" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A8" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A8" s="54"/>
       <c r="B8" s="54" t="s">
         <v>1065</v>
       </c>
@@ -5616,7 +5603,7 @@
       <c r="I8" s="54" t="s">
         <v>343</v>
       </c>
-      <c r="J8" s="68" t="s">
+      <c r="J8" s="67" t="s">
         <v>321</v>
       </c>
       <c r="K8" s="55" t="str">
@@ -5626,10 +5613,10 @@
       <c r="L8" s="55" t="s">
         <v>1154</v>
       </c>
-      <c r="M8" s="75" t="s">
+      <c r="M8" s="74" t="s">
         <v>981</v>
       </c>
-      <c r="N8" s="75" t="s">
+      <c r="N8" s="74" t="s">
         <v>949</v>
       </c>
       <c r="O8" s="61" t="s">
@@ -5643,9 +5630,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A9" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A9" s="54"/>
       <c r="B9" s="54" t="s">
         <v>1066</v>
       </c>
@@ -5670,7 +5655,7 @@
       <c r="I9" s="54" t="s">
         <v>344</v>
       </c>
-      <c r="J9" s="68" t="s">
+      <c r="J9" s="67" t="s">
         <v>322</v>
       </c>
       <c r="K9" s="55" t="str">
@@ -5680,10 +5665,10 @@
       <c r="L9" s="55" t="s">
         <v>1155</v>
       </c>
-      <c r="M9" s="75" t="s">
+      <c r="M9" s="74" t="s">
         <v>982</v>
       </c>
-      <c r="N9" s="75" t="s">
+      <c r="N9" s="74" t="s">
         <v>950</v>
       </c>
       <c r="O9" s="61" t="s">
@@ -5697,9 +5682,7 @@
       </c>
     </row>
     <row r="10" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A10" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A10" s="54"/>
       <c r="B10" s="54" t="s">
         <v>1067</v>
       </c>
@@ -5724,7 +5707,7 @@
       <c r="I10" s="54" t="s">
         <v>341</v>
       </c>
-      <c r="J10" s="68" t="s">
+      <c r="J10" s="67" t="s">
         <v>323</v>
       </c>
       <c r="K10" s="55" t="str">
@@ -5734,10 +5717,10 @@
       <c r="L10" s="55" t="s">
         <v>1156</v>
       </c>
-      <c r="M10" s="75" t="s">
+      <c r="M10" s="74" t="s">
         <v>983</v>
       </c>
-      <c r="N10" s="75" t="s">
+      <c r="N10" s="74" t="s">
         <v>951</v>
       </c>
       <c r="O10" s="61" t="s">
@@ -5751,9 +5734,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A11" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A11" s="54"/>
       <c r="B11" s="54" t="s">
         <v>1068</v>
       </c>
@@ -5778,7 +5759,7 @@
       <c r="I11" s="54" t="s">
         <v>342</v>
       </c>
-      <c r="J11" s="68" t="s">
+      <c r="J11" s="67" t="s">
         <v>324</v>
       </c>
       <c r="K11" s="55" t="str">
@@ -5788,10 +5769,10 @@
       <c r="L11" s="55" t="s">
         <v>1157</v>
       </c>
-      <c r="M11" s="75" t="s">
+      <c r="M11" s="74" t="s">
         <v>336</v>
       </c>
-      <c r="N11" s="75" t="s">
+      <c r="N11" s="74" t="s">
         <v>325</v>
       </c>
       <c r="O11" s="61" t="s">
@@ -5805,9 +5786,7 @@
       </c>
     </row>
     <row r="12" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A12" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A12" s="54"/>
       <c r="B12" s="54" t="s">
         <v>1069</v>
       </c>
@@ -5832,7 +5811,7 @@
       <c r="I12" s="54" t="s">
         <v>345</v>
       </c>
-      <c r="J12" s="68" t="s">
+      <c r="J12" s="67" t="s">
         <v>338</v>
       </c>
       <c r="K12" s="55" t="str">
@@ -5842,8 +5821,8 @@
       <c r="L12" s="55" t="s">
         <v>1158</v>
       </c>
-      <c r="M12" s="75"/>
-      <c r="N12" s="75"/>
+      <c r="M12" s="74"/>
+      <c r="N12" s="74"/>
       <c r="O12" s="61" t="s">
         <v>359</v>
       </c>
@@ -5855,9 +5834,7 @@
       </c>
     </row>
     <row r="13" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A13" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A13" s="54"/>
       <c r="B13" s="54" t="s">
         <v>1070</v>
       </c>
@@ -5882,7 +5859,7 @@
       <c r="I13" s="54" t="s">
         <v>636</v>
       </c>
-      <c r="J13" s="68" t="s">
+      <c r="J13" s="67" t="s">
         <v>634</v>
       </c>
       <c r="K13" s="55" t="str">
@@ -5892,10 +5869,10 @@
       <c r="L13" s="55" t="s">
         <v>1159</v>
       </c>
-      <c r="M13" s="75" t="s">
+      <c r="M13" s="74" t="s">
         <v>780</v>
       </c>
-      <c r="N13" s="75"/>
+      <c r="N13" s="74"/>
       <c r="O13" s="62" t="s">
         <v>780</v>
       </c>
@@ -5905,9 +5882,7 @@
       </c>
     </row>
     <row r="14" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A14" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A14" s="54"/>
       <c r="B14" s="54" t="s">
         <v>1071</v>
       </c>
@@ -5932,7 +5907,7 @@
       <c r="I14" s="54" t="s">
         <v>637</v>
       </c>
-      <c r="J14" s="68" t="s">
+      <c r="J14" s="67" t="s">
         <v>635</v>
       </c>
       <c r="K14" s="55" t="str">
@@ -5942,8 +5917,8 @@
       <c r="L14" s="55" t="s">
         <v>1160</v>
       </c>
-      <c r="M14" s="75"/>
-      <c r="N14" s="75"/>
+      <c r="M14" s="74"/>
+      <c r="N14" s="74"/>
       <c r="O14" s="56" t="s">
         <v>890</v>
       </c>
@@ -5953,9 +5928,7 @@
       </c>
     </row>
     <row r="15" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A15" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A15" s="54"/>
       <c r="B15" s="54" t="s">
         <v>1072</v>
       </c>
@@ -5980,7 +5953,7 @@
       <c r="I15" s="54" t="s">
         <v>775</v>
       </c>
-      <c r="J15" s="68" t="s">
+      <c r="J15" s="67" t="s">
         <v>777</v>
       </c>
       <c r="K15" s="55" t="str">
@@ -5990,8 +5963,8 @@
       <c r="L15" s="55" t="s">
         <v>1161</v>
       </c>
-      <c r="M15" s="75"/>
-      <c r="N15" s="75"/>
+      <c r="M15" s="74"/>
+      <c r="N15" s="74"/>
       <c r="O15" s="56" t="s">
         <v>802</v>
       </c>
@@ -6001,9 +5974,7 @@
       </c>
     </row>
     <row r="16" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A16" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A16" s="54"/>
       <c r="B16" s="54" t="s">
         <v>1073</v>
       </c>
@@ -6028,7 +5999,7 @@
       <c r="I16" s="54" t="s">
         <v>776</v>
       </c>
-      <c r="J16" s="68" t="s">
+      <c r="J16" s="67" t="s">
         <v>778</v>
       </c>
       <c r="K16" s="55" t="str">
@@ -6038,8 +6009,8 @@
       <c r="L16" s="55" t="s">
         <v>1162</v>
       </c>
-      <c r="M16" s="75"/>
-      <c r="N16" s="75"/>
+      <c r="M16" s="74"/>
+      <c r="N16" s="74"/>
       <c r="O16" s="56" t="s">
         <v>802</v>
       </c>
@@ -6049,9 +6020,7 @@
       </c>
     </row>
     <row r="17" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A17" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A17" s="54"/>
       <c r="B17" s="54" t="s">
         <v>1074</v>
       </c>
@@ -6076,7 +6045,7 @@
       <c r="I17" s="54" t="s">
         <v>629</v>
       </c>
-      <c r="J17" s="68" t="str">
+      <c r="J17" s="67" t="str">
         <f t="shared" ref="J17" si="1">CONCATENATE("{""xpath"":[{ ""field"":""/MCCI_IN200100UV01/PORR_IN049006UV/controlActProcess/subject/investigationEvent/component/adverseEventAssessment/subject1/primaryRole/player2/code/@code"",""value"":""",I17,"""}]}")</f>
         <v>{"xpath":[{ "field":"/MCCI_IN200100UV01/PORR_IN049006UV/controlActProcess/subject/investigationEvent/component/adverseEventAssessment/subject1/primaryRole/player2/code/@code","value":"ZEB"}]}</v>
       </c>
@@ -6087,10 +6056,10 @@
       <c r="L17" s="55" t="s">
         <v>1163</v>
       </c>
-      <c r="M17" s="75" t="s">
+      <c r="M17" s="74" t="s">
         <v>984</v>
       </c>
-      <c r="N17" s="75" t="s">
+      <c r="N17" s="74" t="s">
         <v>952</v>
       </c>
       <c r="O17" s="56" t="s">
@@ -6104,9 +6073,7 @@
       </c>
     </row>
     <row r="18" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A18" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A18" s="54"/>
       <c r="B18" s="54" t="s">
         <v>1075</v>
       </c>
@@ -6131,7 +6098,7 @@
       <c r="I18" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="J18" s="68" t="str">
+      <c r="J18" s="67" t="str">
         <f>CONCATENATE("{""xpath"":[{ ""field"":""/MCCI_IN200100UV01/PORR_IN049006UV/controlActProcess/subject/investigationEvent/component/adverseEventAssessment/subject1/primaryRole/player2/code/@code"",""value"":""",I18,"""}]}")</f>
         <v>{"xpath":[{ "field":"/MCCI_IN200100UV01/PORR_IN049006UV/controlActProcess/subject/investigationEvent/component/adverseEventAssessment/subject1/primaryRole/player2/code/@code","value":"invalid"}]}</v>
       </c>
@@ -6142,10 +6109,10 @@
       <c r="L18" s="55" t="s">
         <v>1164</v>
       </c>
-      <c r="M18" s="75" t="s">
+      <c r="M18" s="74" t="s">
         <v>773</v>
       </c>
-      <c r="N18" s="75" t="s">
+      <c r="N18" s="74" t="s">
         <v>365</v>
       </c>
       <c r="O18" s="56" t="s">
@@ -6159,9 +6126,7 @@
       </c>
     </row>
     <row r="19" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A19" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A19" s="54"/>
       <c r="B19" s="54" t="s">
         <v>1076</v>
       </c>
@@ -6186,7 +6151,7 @@
       <c r="I19" s="54" t="s">
         <v>788</v>
       </c>
-      <c r="J19" s="68" t="s">
+      <c r="J19" s="67" t="s">
         <v>784</v>
       </c>
       <c r="K19" s="55" t="str">
@@ -6196,10 +6161,10 @@
       <c r="L19" s="55" t="s">
         <v>1165</v>
       </c>
-      <c r="M19" s="75" t="s">
+      <c r="M19" s="74" t="s">
         <v>985</v>
       </c>
-      <c r="N19" s="75" t="s">
+      <c r="N19" s="74" t="s">
         <v>953</v>
       </c>
       <c r="O19" s="56" t="s">
@@ -6213,9 +6178,7 @@
       </c>
     </row>
     <row r="20" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A20" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A20" s="54"/>
       <c r="B20" s="54" t="s">
         <v>1077</v>
       </c>
@@ -6240,7 +6203,7 @@
       <c r="I20" s="54" t="s">
         <v>789</v>
       </c>
-      <c r="J20" s="68" t="s">
+      <c r="J20" s="67" t="s">
         <v>785</v>
       </c>
       <c r="K20" s="55" t="str">
@@ -6250,10 +6213,10 @@
       <c r="L20" s="55" t="s">
         <v>1166</v>
       </c>
-      <c r="M20" s="75" t="s">
+      <c r="M20" s="74" t="s">
         <v>986</v>
       </c>
-      <c r="N20" s="75" t="s">
+      <c r="N20" s="74" t="s">
         <v>954</v>
       </c>
       <c r="O20" s="56" t="s">
@@ -6267,9 +6230,7 @@
       </c>
     </row>
     <row r="21" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A21" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A21" s="54"/>
       <c r="B21" s="54" t="s">
         <v>1078</v>
       </c>
@@ -6294,7 +6255,7 @@
       <c r="I21" s="54" t="s">
         <v>790</v>
       </c>
-      <c r="J21" s="68" t="s">
+      <c r="J21" s="67" t="s">
         <v>786</v>
       </c>
       <c r="K21" s="55" t="str">
@@ -6304,10 +6265,10 @@
       <c r="L21" s="55" t="s">
         <v>1167</v>
       </c>
-      <c r="M21" s="75" t="s">
+      <c r="M21" s="74" t="s">
         <v>987</v>
       </c>
-      <c r="N21" s="75" t="s">
+      <c r="N21" s="74" t="s">
         <v>955</v>
       </c>
       <c r="O21" s="56" t="s">
@@ -6321,9 +6282,7 @@
       </c>
     </row>
     <row r="22" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A22" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A22" s="54"/>
       <c r="B22" s="54" t="s">
         <v>1079</v>
       </c>
@@ -6348,7 +6307,7 @@
       <c r="I22" s="54" t="s">
         <v>791</v>
       </c>
-      <c r="J22" s="68" t="s">
+      <c r="J22" s="67" t="s">
         <v>787</v>
       </c>
       <c r="K22" s="55" t="str">
@@ -6358,10 +6317,10 @@
       <c r="L22" s="55" t="s">
         <v>1168</v>
       </c>
-      <c r="M22" s="75" t="s">
+      <c r="M22" s="74" t="s">
         <v>800</v>
       </c>
-      <c r="N22" s="75" t="s">
+      <c r="N22" s="74" t="s">
         <v>806</v>
       </c>
       <c r="O22" s="56" t="s">
@@ -6375,9 +6334,7 @@
       </c>
     </row>
     <row r="23" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A23" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A23" s="54"/>
       <c r="B23" s="54" t="s">
         <v>1080</v>
       </c>
@@ -6402,7 +6359,7 @@
       <c r="I23" s="54" t="s">
         <v>792</v>
       </c>
-      <c r="J23" s="68" t="s">
+      <c r="J23" s="67" t="s">
         <v>793</v>
       </c>
       <c r="K23" s="55" t="str">
@@ -6412,10 +6369,10 @@
       <c r="L23" s="55" t="s">
         <v>1169</v>
       </c>
-      <c r="M23" s="75" t="s">
+      <c r="M23" s="74" t="s">
         <v>800</v>
       </c>
-      <c r="N23" s="75" t="s">
+      <c r="N23" s="74" t="s">
         <v>806</v>
       </c>
       <c r="O23" s="56" t="s">
@@ -6429,9 +6386,7 @@
       </c>
     </row>
     <row r="24" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A24" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A24" s="54"/>
       <c r="B24" s="54" t="s">
         <v>1081</v>
       </c>
@@ -6456,7 +6411,7 @@
       <c r="I24" s="54" t="s">
         <v>346</v>
       </c>
-      <c r="J24" s="68" t="s">
+      <c r="J24" s="67" t="s">
         <v>795</v>
       </c>
       <c r="K24" s="55" t="str">
@@ -6466,13 +6421,13 @@
       <c r="L24" s="55" t="s">
         <v>1170</v>
       </c>
-      <c r="M24" s="75" t="s">
+      <c r="M24" s="74" t="s">
         <v>1013</v>
       </c>
-      <c r="N24" s="75" t="s">
+      <c r="N24" s="74" t="s">
         <v>1013</v>
       </c>
-      <c r="O24" s="76" t="s">
+      <c r="O24" s="75" t="s">
         <v>1013</v>
       </c>
       <c r="P24" s="62" t="s">
@@ -6483,9 +6438,7 @@
       </c>
     </row>
     <row r="25" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A25" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A25" s="54"/>
       <c r="B25" s="54" t="s">
         <v>1082</v>
       </c>
@@ -6510,7 +6463,7 @@
       <c r="I25" s="54" t="s">
         <v>794</v>
       </c>
-      <c r="J25" s="68" t="s">
+      <c r="J25" s="67" t="s">
         <v>783</v>
       </c>
       <c r="K25" s="55" t="str">
@@ -6520,13 +6473,13 @@
       <c r="L25" s="55" t="s">
         <v>1171</v>
       </c>
-      <c r="M25" s="75" t="s">
+      <c r="M25" s="74" t="s">
         <v>1013</v>
       </c>
-      <c r="N25" s="75" t="s">
+      <c r="N25" s="74" t="s">
         <v>1013</v>
       </c>
-      <c r="O25" s="76" t="s">
+      <c r="O25" s="75" t="s">
         <v>1013</v>
       </c>
       <c r="P25" s="62" t="s">
@@ -6537,9 +6490,7 @@
       </c>
     </row>
     <row r="26" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A26" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A26" s="54"/>
       <c r="B26" s="54" t="s">
         <v>1083</v>
       </c>
@@ -6564,7 +6515,7 @@
       <c r="I26" s="54" t="s">
         <v>810</v>
       </c>
-      <c r="J26" s="68" t="s">
+      <c r="J26" s="67" t="s">
         <v>808</v>
       </c>
       <c r="K26" s="55" t="str">
@@ -6574,10 +6525,10 @@
       <c r="L26" s="55" t="s">
         <v>1172</v>
       </c>
-      <c r="M26" s="75" t="s">
+      <c r="M26" s="74" t="s">
         <v>988</v>
       </c>
-      <c r="N26" s="75" t="s">
+      <c r="N26" s="74" t="s">
         <v>956</v>
       </c>
       <c r="O26" s="56" t="s">
@@ -6591,9 +6542,7 @@
       </c>
     </row>
     <row r="27" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A27" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A27" s="54"/>
       <c r="B27" s="54" t="s">
         <v>1084</v>
       </c>
@@ -6618,7 +6567,7 @@
       <c r="I27" s="54" t="s">
         <v>811</v>
       </c>
-      <c r="J27" s="68" t="s">
+      <c r="J27" s="67" t="s">
         <v>812</v>
       </c>
       <c r="K27" s="55" t="str">
@@ -6645,9 +6594,7 @@
       </c>
     </row>
     <row r="28" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A28" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A28" s="54"/>
       <c r="B28" s="54" t="s">
         <v>1085</v>
       </c>
@@ -6672,7 +6619,7 @@
       <c r="I28" s="54" t="s">
         <v>813</v>
       </c>
-      <c r="J28" s="68" t="s">
+      <c r="J28" s="67" t="s">
         <v>814</v>
       </c>
       <c r="K28" s="55" t="str">
@@ -6682,10 +6629,10 @@
       <c r="L28" s="55" t="s">
         <v>1174</v>
       </c>
-      <c r="M28" s="75" t="s">
+      <c r="M28" s="74" t="s">
         <v>984</v>
       </c>
-      <c r="N28" s="75" t="s">
+      <c r="N28" s="74" t="s">
         <v>952</v>
       </c>
       <c r="O28" s="56" t="s">
@@ -6699,9 +6646,7 @@
       </c>
     </row>
     <row r="29" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A29" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A29" s="54"/>
       <c r="B29" s="54" t="s">
         <v>1086</v>
       </c>
@@ -6726,7 +6671,7 @@
       <c r="I29" s="54" t="s">
         <v>815</v>
       </c>
-      <c r="J29" s="68" t="s">
+      <c r="J29" s="67" t="s">
         <v>816</v>
       </c>
       <c r="K29" s="55" t="str">
@@ -6736,10 +6681,10 @@
       <c r="L29" s="55" t="s">
         <v>1175</v>
       </c>
-      <c r="M29" s="75" t="s">
+      <c r="M29" s="74" t="s">
         <v>990</v>
       </c>
-      <c r="N29" s="75" t="s">
+      <c r="N29" s="74" t="s">
         <v>958</v>
       </c>
       <c r="O29" s="56" t="s">
@@ -6753,9 +6698,7 @@
       </c>
     </row>
     <row r="30" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A30" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A30" s="54"/>
       <c r="B30" s="54" t="s">
         <v>1087</v>
       </c>
@@ -6780,7 +6723,7 @@
       <c r="I30" s="54" t="s">
         <v>818</v>
       </c>
-      <c r="J30" s="68" t="s">
+      <c r="J30" s="67" t="s">
         <v>817</v>
       </c>
       <c r="K30" s="55" t="str">
@@ -6790,10 +6733,10 @@
       <c r="L30" s="55" t="s">
         <v>1176</v>
       </c>
-      <c r="M30" s="75" t="s">
+      <c r="M30" s="74" t="s">
         <v>989</v>
       </c>
-      <c r="N30" s="75" t="s">
+      <c r="N30" s="74" t="s">
         <v>957</v>
       </c>
       <c r="O30" s="56" t="s">
@@ -6807,9 +6750,7 @@
       </c>
     </row>
     <row r="31" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A31" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A31" s="54"/>
       <c r="B31" s="54" t="s">
         <v>1088</v>
       </c>
@@ -6834,7 +6775,7 @@
       <c r="I31" s="54" t="s">
         <v>819</v>
       </c>
-      <c r="J31" s="68" t="s">
+      <c r="J31" s="67" t="s">
         <v>820</v>
       </c>
       <c r="K31" s="55" t="str">
@@ -6844,10 +6785,10 @@
       <c r="L31" s="55" t="s">
         <v>1177</v>
       </c>
-      <c r="M31" s="75" t="s">
+      <c r="M31" s="74" t="s">
         <v>991</v>
       </c>
-      <c r="N31" s="75" t="s">
+      <c r="N31" s="74" t="s">
         <v>959</v>
       </c>
       <c r="O31" s="56" t="s">
@@ -6861,9 +6802,7 @@
       </c>
     </row>
     <row r="32" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A32" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A32" s="54"/>
       <c r="B32" s="54" t="s">
         <v>1089</v>
       </c>
@@ -6888,7 +6827,7 @@
       <c r="I32" s="54" t="s">
         <v>821</v>
       </c>
-      <c r="J32" s="68" t="s">
+      <c r="J32" s="67" t="s">
         <v>822</v>
       </c>
       <c r="K32" s="55" t="str">
@@ -6898,10 +6837,10 @@
       <c r="L32" s="55" t="s">
         <v>1178</v>
       </c>
-      <c r="M32" s="75" t="s">
+      <c r="M32" s="74" t="s">
         <v>992</v>
       </c>
-      <c r="N32" s="75" t="s">
+      <c r="N32" s="74" t="s">
         <v>960</v>
       </c>
       <c r="O32" s="56" t="s">
@@ -6915,9 +6854,7 @@
       </c>
     </row>
     <row r="33" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A33" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A33" s="54"/>
       <c r="B33" s="54" t="s">
         <v>1090</v>
       </c>
@@ -6942,7 +6879,7 @@
       <c r="I33" s="54" t="s">
         <v>826</v>
       </c>
-      <c r="J33" s="68" t="s">
+      <c r="J33" s="67" t="s">
         <v>824</v>
       </c>
       <c r="K33" s="55" t="str">
@@ -6952,10 +6889,10 @@
       <c r="L33" s="55" t="s">
         <v>1179</v>
       </c>
-      <c r="M33" s="75" t="s">
+      <c r="M33" s="74" t="s">
         <v>989</v>
       </c>
-      <c r="N33" s="75" t="s">
+      <c r="N33" s="74" t="s">
         <v>957</v>
       </c>
       <c r="O33" s="56" t="s">
@@ -6969,9 +6906,7 @@
       </c>
     </row>
     <row r="34" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A34" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A34" s="54"/>
       <c r="B34" s="54" t="s">
         <v>1091</v>
       </c>
@@ -6996,7 +6931,7 @@
       <c r="I34" s="54" t="s">
         <v>825</v>
       </c>
-      <c r="J34" s="68" t="s">
+      <c r="J34" s="67" t="s">
         <v>809</v>
       </c>
       <c r="K34" s="55" t="str">
@@ -7006,8 +6941,8 @@
       <c r="L34" s="55" t="s">
         <v>1180</v>
       </c>
-      <c r="M34" s="75"/>
-      <c r="N34" s="75"/>
+      <c r="M34" s="74"/>
+      <c r="N34" s="74"/>
       <c r="O34" s="56" t="s">
         <v>883</v>
       </c>
@@ -7017,9 +6952,7 @@
       </c>
     </row>
     <row r="35" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A35" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A35" s="54"/>
       <c r="B35" s="54" t="s">
         <v>1092</v>
       </c>
@@ -7044,7 +6977,7 @@
       <c r="I35" s="54" t="s">
         <v>827</v>
       </c>
-      <c r="J35" s="68" t="s">
+      <c r="J35" s="67" t="s">
         <v>828</v>
       </c>
       <c r="K35" s="55" t="str">
@@ -7054,8 +6987,8 @@
       <c r="L35" s="55" t="s">
         <v>1181</v>
       </c>
-      <c r="M35" s="75"/>
-      <c r="N35" s="75"/>
+      <c r="M35" s="74"/>
+      <c r="N35" s="74"/>
       <c r="O35" s="56" t="s">
         <v>883</v>
       </c>
@@ -7065,9 +6998,7 @@
       </c>
     </row>
     <row r="36" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A36" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A36" s="54"/>
       <c r="B36" s="54" t="s">
         <v>1093</v>
       </c>
@@ -7092,7 +7023,7 @@
       <c r="I36" s="54" t="s">
         <v>842</v>
       </c>
-      <c r="J36" s="68" t="s">
+      <c r="J36" s="67" t="s">
         <v>843</v>
       </c>
       <c r="K36" s="55" t="str">
@@ -7102,8 +7033,8 @@
       <c r="L36" s="55" t="s">
         <v>1182</v>
       </c>
-      <c r="M36" s="75"/>
-      <c r="N36" s="75"/>
+      <c r="M36" s="74"/>
+      <c r="N36" s="74"/>
       <c r="O36" s="56" t="s">
         <v>883</v>
       </c>
@@ -7113,9 +7044,7 @@
       </c>
     </row>
     <row r="37" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A37" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A37" s="54"/>
       <c r="B37" s="54" t="s">
         <v>1094</v>
       </c>
@@ -7140,7 +7069,7 @@
       <c r="I37" s="54" t="s">
         <v>879</v>
       </c>
-      <c r="J37" s="68" t="s">
+      <c r="J37" s="67" t="s">
         <v>847</v>
       </c>
       <c r="K37" s="55" t="str">
@@ -7150,8 +7079,8 @@
       <c r="L37" s="55" t="s">
         <v>1183</v>
       </c>
-      <c r="M37" s="75"/>
-      <c r="N37" s="75"/>
+      <c r="M37" s="74"/>
+      <c r="N37" s="74"/>
       <c r="O37" s="56" t="s">
         <v>63</v>
       </c>
@@ -7163,9 +7092,7 @@
       </c>
     </row>
     <row r="38" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A38" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A38" s="54"/>
       <c r="B38" s="54" t="s">
         <v>1095</v>
       </c>
@@ -7190,7 +7117,7 @@
       <c r="I38" s="54" t="s">
         <v>880</v>
       </c>
-      <c r="J38" s="68" t="s">
+      <c r="J38" s="67" t="s">
         <v>854</v>
       </c>
       <c r="K38" s="55" t="str">
@@ -7200,8 +7127,8 @@
       <c r="L38" s="55" t="s">
         <v>1184</v>
       </c>
-      <c r="M38" s="75"/>
-      <c r="N38" s="75"/>
+      <c r="M38" s="74"/>
+      <c r="N38" s="74"/>
       <c r="O38" s="56" t="s">
         <v>63</v>
       </c>
@@ -7213,9 +7140,7 @@
       </c>
     </row>
     <row r="39" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A39" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A39" s="54"/>
       <c r="B39" s="54" t="s">
         <v>1096</v>
       </c>
@@ -7240,7 +7165,7 @@
       <c r="I39" s="54" t="s">
         <v>855</v>
       </c>
-      <c r="J39" s="68" t="s">
+      <c r="J39" s="67" t="s">
         <v>857</v>
       </c>
       <c r="K39" s="55" t="str">
@@ -7250,8 +7175,8 @@
       <c r="L39" s="55" t="s">
         <v>1185</v>
       </c>
-      <c r="M39" s="75"/>
-      <c r="N39" s="75"/>
+      <c r="M39" s="74"/>
+      <c r="N39" s="74"/>
       <c r="O39" s="56" t="s">
         <v>867</v>
       </c>
@@ -7261,9 +7186,7 @@
       </c>
     </row>
     <row r="40" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A40" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A40" s="54"/>
       <c r="B40" s="54" t="s">
         <v>1097</v>
       </c>
@@ -7288,7 +7211,7 @@
       <c r="I40" s="54" t="s">
         <v>856</v>
       </c>
-      <c r="J40" s="68" t="s">
+      <c r="J40" s="67" t="s">
         <v>849</v>
       </c>
       <c r="K40" s="55" t="str">
@@ -7298,8 +7221,8 @@
       <c r="L40" s="55" t="s">
         <v>1186</v>
       </c>
-      <c r="M40" s="75"/>
-      <c r="N40" s="75"/>
+      <c r="M40" s="74"/>
+      <c r="N40" s="74"/>
       <c r="O40" s="56" t="s">
         <v>867</v>
       </c>
@@ -7309,9 +7232,7 @@
       </c>
     </row>
     <row r="41" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A41" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A41" s="54"/>
       <c r="B41" s="54" t="s">
         <v>1098</v>
       </c>
@@ -7336,7 +7257,7 @@
       <c r="I41" s="54" t="s">
         <v>848</v>
       </c>
-      <c r="J41" s="68" t="s">
+      <c r="J41" s="67" t="s">
         <v>850</v>
       </c>
       <c r="K41" s="55" t="str">
@@ -7346,10 +7267,10 @@
       <c r="L41" s="55" t="s">
         <v>1187</v>
       </c>
-      <c r="M41" s="75" t="s">
+      <c r="M41" s="74" t="s">
         <v>993</v>
       </c>
-      <c r="N41" s="75" t="s">
+      <c r="N41" s="74" t="s">
         <v>961</v>
       </c>
       <c r="O41" s="56"/>
@@ -7361,9 +7282,7 @@
       </c>
     </row>
     <row r="42" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A42" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A42" s="54"/>
       <c r="B42" s="54" t="s">
         <v>1099</v>
       </c>
@@ -7388,7 +7307,7 @@
       <c r="I42" s="54" t="s">
         <v>848</v>
       </c>
-      <c r="J42" s="68" t="s">
+      <c r="J42" s="67" t="s">
         <v>851</v>
       </c>
       <c r="K42" s="55" t="str">
@@ -7398,10 +7317,10 @@
       <c r="L42" s="55" t="s">
         <v>1188</v>
       </c>
-      <c r="M42" s="75" t="s">
+      <c r="M42" s="74" t="s">
         <v>994</v>
       </c>
-      <c r="N42" s="75" t="s">
+      <c r="N42" s="74" t="s">
         <v>962</v>
       </c>
       <c r="O42" s="56"/>
@@ -7413,9 +7332,7 @@
       </c>
     </row>
     <row r="43" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A43" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A43" s="54"/>
       <c r="B43" s="54" t="s">
         <v>1100</v>
       </c>
@@ -7440,7 +7357,7 @@
       <c r="I43" s="54" t="s">
         <v>848</v>
       </c>
-      <c r="J43" s="68" t="s">
+      <c r="J43" s="67" t="s">
         <v>852</v>
       </c>
       <c r="K43" s="55" t="str">
@@ -7450,10 +7367,10 @@
       <c r="L43" s="55" t="s">
         <v>1189</v>
       </c>
-      <c r="M43" s="75" t="s">
+      <c r="M43" s="74" t="s">
         <v>995</v>
       </c>
-      <c r="N43" s="75" t="s">
+      <c r="N43" s="74" t="s">
         <v>963</v>
       </c>
       <c r="O43" s="56"/>
@@ -7465,9 +7382,7 @@
       </c>
     </row>
     <row r="44" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A44" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A44" s="54"/>
       <c r="B44" s="54" t="s">
         <v>1101</v>
       </c>
@@ -7492,7 +7407,7 @@
       <c r="I44" s="54" t="s">
         <v>848</v>
       </c>
-      <c r="J44" s="68" t="s">
+      <c r="J44" s="67" t="s">
         <v>853</v>
       </c>
       <c r="K44" s="55" t="str">
@@ -7502,10 +7417,10 @@
       <c r="L44" s="55" t="s">
         <v>1190</v>
       </c>
-      <c r="M44" s="75" t="s">
+      <c r="M44" s="74" t="s">
         <v>996</v>
       </c>
-      <c r="N44" s="75"/>
+      <c r="N44" s="74"/>
       <c r="O44" s="56" t="s">
         <v>885</v>
       </c>
@@ -7517,9 +7432,7 @@
       </c>
     </row>
     <row r="45" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A45" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A45" s="54"/>
       <c r="B45" s="54" t="s">
         <v>1102</v>
       </c>
@@ -7544,7 +7457,7 @@
       <c r="I45" s="54" t="s">
         <v>848</v>
       </c>
-      <c r="J45" s="68" t="s">
+      <c r="J45" s="67" t="s">
         <v>882</v>
       </c>
       <c r="K45" s="55" t="str">
@@ -7554,10 +7467,10 @@
       <c r="L45" s="55" t="s">
         <v>1191</v>
       </c>
-      <c r="M45" s="75" t="s">
+      <c r="M45" s="74" t="s">
         <v>996</v>
       </c>
-      <c r="N45" s="75"/>
+      <c r="N45" s="74"/>
       <c r="O45" s="56" t="s">
         <v>916</v>
       </c>
@@ -7569,9 +7482,7 @@
       </c>
     </row>
     <row r="46" spans="1:17" s="57" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A46" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A46" s="54"/>
       <c r="B46" s="54" t="s">
         <v>1103</v>
       </c>
@@ -7596,7 +7507,7 @@
       <c r="I46" s="54" t="s">
         <v>886</v>
       </c>
-      <c r="J46" s="68" t="s">
+      <c r="J46" s="67" t="s">
         <v>859</v>
       </c>
       <c r="K46" s="55" t="str">
@@ -7606,8 +7517,8 @@
       <c r="L46" s="55" t="s">
         <v>1192</v>
       </c>
-      <c r="M46" s="75"/>
-      <c r="N46" s="75"/>
+      <c r="M46" s="74"/>
+      <c r="N46" s="74"/>
       <c r="O46" s="57" t="s">
         <v>888</v>
       </c>
@@ -7619,9 +7530,7 @@
       </c>
     </row>
     <row r="47" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A47" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A47" s="54"/>
       <c r="B47" s="54" t="s">
         <v>1104</v>
       </c>
@@ -7646,7 +7555,7 @@
       <c r="I47" s="54" t="s">
         <v>887</v>
       </c>
-      <c r="J47" s="68" t="s">
+      <c r="J47" s="67" t="s">
         <v>860</v>
       </c>
       <c r="K47" s="55" t="str">
@@ -7656,16 +7565,14 @@
       <c r="L47" s="55" t="s">
         <v>1193</v>
       </c>
-      <c r="M47" s="75"/>
-      <c r="N47" s="75"/>
+      <c r="M47" s="74"/>
+      <c r="N47" s="74"/>
       <c r="P47" s="61" t="s">
         <v>867</v>
       </c>
     </row>
     <row r="48" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A48" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A48" s="54"/>
       <c r="B48" s="54" t="s">
         <v>1105</v>
       </c>
@@ -7690,7 +7597,7 @@
       <c r="I48" s="54" t="s">
         <v>862</v>
       </c>
-      <c r="J48" s="68" t="s">
+      <c r="J48" s="67" t="s">
         <v>868</v>
       </c>
       <c r="K48" s="55" t="str">
@@ -7700,10 +7607,10 @@
       <c r="L48" s="55" t="s">
         <v>1194</v>
       </c>
-      <c r="M48" s="75" t="s">
+      <c r="M48" s="74" t="s">
         <v>997</v>
       </c>
-      <c r="N48" s="75" t="s">
+      <c r="N48" s="74" t="s">
         <v>964</v>
       </c>
       <c r="P48" s="62" t="s">
@@ -7711,9 +7618,7 @@
       </c>
     </row>
     <row r="49" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A49" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A49" s="54"/>
       <c r="B49" s="54" t="s">
         <v>1106</v>
       </c>
@@ -7738,7 +7643,7 @@
       <c r="I49" s="54" t="s">
         <v>863</v>
       </c>
-      <c r="J49" s="68" t="s">
+      <c r="J49" s="67" t="s">
         <v>869</v>
       </c>
       <c r="K49" s="55" t="str">
@@ -7748,8 +7653,8 @@
       <c r="L49" s="55" t="s">
         <v>1195</v>
       </c>
-      <c r="M49" s="75"/>
-      <c r="N49" s="75"/>
+      <c r="M49" s="74"/>
+      <c r="N49" s="74"/>
       <c r="O49" s="56" t="s">
         <v>891</v>
       </c>
@@ -7761,9 +7666,7 @@
       </c>
     </row>
     <row r="50" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A50" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A50" s="54"/>
       <c r="B50" s="54" t="s">
         <v>1107</v>
       </c>
@@ -7788,7 +7691,7 @@
       <c r="I50" s="54" t="s">
         <v>863</v>
       </c>
-      <c r="J50" s="68" t="s">
+      <c r="J50" s="67" t="s">
         <v>870</v>
       </c>
       <c r="K50" s="55" t="str">
@@ -7798,8 +7701,8 @@
       <c r="L50" s="55" t="s">
         <v>1196</v>
       </c>
-      <c r="M50" s="75"/>
-      <c r="N50" s="75"/>
+      <c r="M50" s="74"/>
+      <c r="N50" s="74"/>
       <c r="O50" s="56" t="s">
         <v>889</v>
       </c>
@@ -7811,9 +7714,7 @@
       </c>
     </row>
     <row r="51" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A51" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A51" s="54"/>
       <c r="B51" s="54" t="s">
         <v>1108</v>
       </c>
@@ -7838,7 +7739,7 @@
       <c r="I51" s="54" t="s">
         <v>863</v>
       </c>
-      <c r="J51" s="68" t="s">
+      <c r="J51" s="67" t="s">
         <v>871</v>
       </c>
       <c r="K51" s="55" t="str">
@@ -7848,8 +7749,8 @@
       <c r="L51" s="55" t="s">
         <v>1197</v>
       </c>
-      <c r="M51" s="75"/>
-      <c r="N51" s="75"/>
+      <c r="M51" s="74"/>
+      <c r="N51" s="74"/>
       <c r="O51" s="56" t="s">
         <v>891</v>
       </c>
@@ -7861,9 +7762,7 @@
       </c>
     </row>
     <row r="52" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A52" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A52" s="54"/>
       <c r="B52" s="54" t="s">
         <v>1109</v>
       </c>
@@ -7888,7 +7787,7 @@
       <c r="I52" s="54" t="s">
         <v>863</v>
       </c>
-      <c r="J52" s="68" t="s">
+      <c r="J52" s="67" t="s">
         <v>872</v>
       </c>
       <c r="K52" s="55" t="str">
@@ -7898,8 +7797,8 @@
       <c r="L52" s="55" t="s">
         <v>1198</v>
       </c>
-      <c r="M52" s="75"/>
-      <c r="N52" s="75"/>
+      <c r="M52" s="74"/>
+      <c r="N52" s="74"/>
       <c r="O52" s="56" t="s">
         <v>891</v>
       </c>
@@ -7911,9 +7810,7 @@
       </c>
     </row>
     <row r="53" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A53" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A53" s="54"/>
       <c r="B53" s="54" t="s">
         <v>1110</v>
       </c>
@@ -7938,7 +7835,7 @@
       <c r="I53" s="54" t="s">
         <v>863</v>
       </c>
-      <c r="J53" s="68" t="s">
+      <c r="J53" s="67" t="s">
         <v>873</v>
       </c>
       <c r="K53" s="55" t="str">
@@ -7948,8 +7845,8 @@
       <c r="L53" s="55" t="s">
         <v>1199</v>
       </c>
-      <c r="M53" s="75"/>
-      <c r="N53" s="75"/>
+      <c r="M53" s="74"/>
+      <c r="N53" s="74"/>
       <c r="O53" s="56" t="s">
         <v>891</v>
       </c>
@@ -7961,9 +7858,7 @@
       </c>
     </row>
     <row r="54" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A54" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A54" s="54"/>
       <c r="B54" s="54" t="s">
         <v>1111</v>
       </c>
@@ -7988,7 +7883,7 @@
       <c r="I54" s="54" t="s">
         <v>865</v>
       </c>
-      <c r="J54" s="68" t="s">
+      <c r="J54" s="67" t="s">
         <v>874</v>
       </c>
       <c r="K54" s="55" t="str">
@@ -7998,8 +7893,8 @@
       <c r="L54" s="55" t="s">
         <v>1200</v>
       </c>
-      <c r="M54" s="75"/>
-      <c r="N54" s="75"/>
+      <c r="M54" s="74"/>
+      <c r="N54" s="74"/>
       <c r="O54" s="56" t="s">
         <v>891</v>
       </c>
@@ -8011,9 +7906,7 @@
       </c>
     </row>
     <row r="55" spans="1:17" s="60" customFormat="1" ht="9.75" customHeight="1">
-      <c r="A55" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A55" s="54"/>
       <c r="B55" s="54" t="s">
         <v>1112</v>
       </c>
@@ -8038,7 +7931,7 @@
       <c r="I55" s="54" t="s">
         <v>864</v>
       </c>
-      <c r="J55" s="68" t="s">
+      <c r="J55" s="67" t="s">
         <v>875</v>
       </c>
       <c r="K55" s="55" t="str">
@@ -8048,10 +7941,10 @@
       <c r="L55" s="55" t="s">
         <v>1201</v>
       </c>
-      <c r="M55" s="75" t="s">
+      <c r="M55" s="74" t="s">
         <v>998</v>
       </c>
-      <c r="N55" s="75" t="s">
+      <c r="N55" s="74" t="s">
         <v>965</v>
       </c>
       <c r="P55" s="62" t="s">
@@ -8062,9 +7955,7 @@
       </c>
     </row>
     <row r="56" spans="1:17" ht="9.75" customHeight="1">
-      <c r="A56" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A56" s="54"/>
       <c r="B56" s="54" t="s">
         <v>1113</v>
       </c>
@@ -8099,10 +7990,10 @@
       <c r="L56" s="55" t="s">
         <v>1202</v>
       </c>
-      <c r="M56" s="75" t="s">
+      <c r="M56" s="74" t="s">
         <v>999</v>
       </c>
-      <c r="N56" s="75"/>
+      <c r="N56" s="74"/>
       <c r="O56" s="49" t="s">
         <v>895</v>
       </c>
@@ -8114,9 +8005,7 @@
       </c>
     </row>
     <row r="57" spans="1:17" ht="9.75" customHeight="1">
-      <c r="A57" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A57" s="54"/>
       <c r="B57" s="54" t="s">
         <v>1114</v>
       </c>
@@ -8151,8 +8040,8 @@
       <c r="L57" s="55" t="s">
         <v>1203</v>
       </c>
-      <c r="M57" s="75"/>
-      <c r="N57" s="75"/>
+      <c r="M57" s="74"/>
+      <c r="N57" s="74"/>
       <c r="O57" s="49" t="s">
         <v>895</v>
       </c>
@@ -8164,9 +8053,7 @@
       </c>
     </row>
     <row r="58" spans="1:17" ht="9.75" customHeight="1">
-      <c r="A58" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A58" s="54"/>
       <c r="B58" s="54" t="s">
         <v>1115</v>
       </c>
@@ -8201,8 +8088,8 @@
       <c r="L58" s="55" t="s">
         <v>1204</v>
       </c>
-      <c r="M58" s="75"/>
-      <c r="N58" s="75"/>
+      <c r="M58" s="74"/>
+      <c r="N58" s="74"/>
       <c r="P58" s="66" t="s">
         <v>867</v>
       </c>
@@ -8211,9 +8098,7 @@
       </c>
     </row>
     <row r="59" spans="1:17" ht="9.75" customHeight="1">
-      <c r="A59" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A59" s="54"/>
       <c r="B59" s="54" t="s">
         <v>1116</v>
       </c>
@@ -8229,7 +8114,7 @@
       <c r="F59" s="54" t="s">
         <v>320</v>
       </c>
-      <c r="G59" s="77">
+      <c r="G59" s="76">
         <v>1</v>
       </c>
       <c r="H59" s="59" t="s">
@@ -8248,10 +8133,10 @@
       <c r="L59" s="55" t="s">
         <v>1205</v>
       </c>
-      <c r="M59" s="75" t="s">
+      <c r="M59" s="74" t="s">
         <v>1000</v>
       </c>
-      <c r="N59" s="75" t="s">
+      <c r="N59" s="74" t="s">
         <v>966</v>
       </c>
       <c r="P59" s="66" t="s">
@@ -8262,9 +8147,7 @@
       </c>
     </row>
     <row r="60" spans="1:17" ht="9.75" customHeight="1">
-      <c r="A60" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A60" s="54"/>
       <c r="B60" s="54" t="s">
         <v>1117</v>
       </c>
@@ -8280,7 +8163,7 @@
       <c r="F60" s="54" t="s">
         <v>320</v>
       </c>
-      <c r="G60" s="77">
+      <c r="G60" s="76">
         <v>59</v>
       </c>
       <c r="H60" s="59" t="s">
@@ -8299,10 +8182,10 @@
       <c r="L60" s="55" t="s">
         <v>1206</v>
       </c>
-      <c r="M60" s="75" t="s">
+      <c r="M60" s="74" t="s">
         <v>1001</v>
       </c>
-      <c r="N60" s="75" t="s">
+      <c r="N60" s="74" t="s">
         <v>967</v>
       </c>
       <c r="P60" s="66" t="s">
@@ -8313,9 +8196,7 @@
       </c>
     </row>
     <row r="61" spans="1:17" ht="9.75" customHeight="1">
-      <c r="A61" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A61" s="54"/>
       <c r="B61" s="54" t="s">
         <v>1118</v>
       </c>
@@ -8331,7 +8212,7 @@
       <c r="F61" s="54" t="s">
         <v>320</v>
       </c>
-      <c r="G61" s="77">
+      <c r="G61" s="76">
         <v>60</v>
       </c>
       <c r="H61" s="59" t="s">
@@ -8350,10 +8231,10 @@
       <c r="L61" s="55" t="s">
         <v>1207</v>
       </c>
-      <c r="M61" s="75" t="s">
+      <c r="M61" s="74" t="s">
         <v>1002</v>
       </c>
-      <c r="N61" s="75" t="s">
+      <c r="N61" s="74" t="s">
         <v>968</v>
       </c>
       <c r="P61" s="66" t="s">
@@ -8364,9 +8245,7 @@
       </c>
     </row>
     <row r="62" spans="1:17" ht="9.75" customHeight="1">
-      <c r="A62" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A62" s="54"/>
       <c r="B62" s="54" t="s">
         <v>1119</v>
       </c>
@@ -8382,7 +8261,7 @@
       <c r="F62" s="54" t="s">
         <v>320</v>
       </c>
-      <c r="G62" s="77">
+      <c r="G62" s="76">
         <v>61</v>
       </c>
       <c r="H62" s="54" t="s">
@@ -8401,10 +8280,10 @@
       <c r="L62" s="55" t="s">
         <v>1208</v>
       </c>
-      <c r="M62" s="75" t="s">
+      <c r="M62" s="74" t="s">
         <v>996</v>
       </c>
-      <c r="N62" s="75"/>
+      <c r="N62" s="74"/>
       <c r="P62" s="66" t="s">
         <v>913</v>
       </c>
@@ -8413,9 +8292,7 @@
       </c>
     </row>
     <row r="63" spans="1:17" ht="9.75" customHeight="1">
-      <c r="A63" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A63" s="54"/>
       <c r="B63" s="54" t="s">
         <v>1120</v>
       </c>
@@ -8431,7 +8308,7 @@
       <c r="F63" s="54" t="s">
         <v>320</v>
       </c>
-      <c r="G63" s="77">
+      <c r="G63" s="76">
         <v>70</v>
       </c>
       <c r="H63" s="54" t="s">
@@ -8450,10 +8327,10 @@
       <c r="L63" s="55" t="s">
         <v>1209</v>
       </c>
-      <c r="M63" s="75" t="s">
+      <c r="M63" s="74" t="s">
         <v>996</v>
       </c>
-      <c r="N63" s="75"/>
+      <c r="N63" s="74"/>
       <c r="P63" s="66" t="s">
         <v>915</v>
       </c>
@@ -8462,25 +8339,23 @@
       </c>
     </row>
     <row r="64" spans="1:17" ht="9.75" customHeight="1">
-      <c r="A64" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A64" s="54"/>
       <c r="B64" s="54" t="s">
         <v>1121</v>
       </c>
       <c r="C64" s="59" t="s">
         <v>917</v>
       </c>
-      <c r="D64" s="71" t="s">
+      <c r="D64" s="70" t="s">
         <v>1039</v>
       </c>
       <c r="E64" s="60">
         <v>198</v>
       </c>
-      <c r="F64" s="71" t="s">
+      <c r="F64" s="70" t="s">
         <v>1038</v>
       </c>
-      <c r="G64" s="71" t="s">
+      <c r="G64" s="70" t="s">
         <v>1040</v>
       </c>
       <c r="H64" s="59" t="s">
@@ -8489,7 +8364,7 @@
       <c r="I64" s="59" t="s">
         <v>918</v>
       </c>
-      <c r="J64" s="70"/>
+      <c r="J64" s="69"/>
       <c r="K64" s="55" t="str">
         <f t="shared" si="0"/>
         <v>TC64_B25_offLabel_198_bizrul_true251null_p</v>
@@ -8497,36 +8372,34 @@
       <c r="L64" s="55" t="s">
         <v>1210</v>
       </c>
-      <c r="M64" s="75" t="s">
+      <c r="M64" s="74" t="s">
         <v>1003</v>
       </c>
-      <c r="N64" s="75" t="s">
+      <c r="N64" s="74" t="s">
         <v>969</v>
       </c>
-      <c r="O64" s="74" t="s">
+      <c r="O64" s="73" t="s">
         <v>931</v>
       </c>
     </row>
     <row r="65" spans="1:15" ht="9.75" customHeight="1">
-      <c r="A65" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A65" s="54"/>
       <c r="B65" s="54" t="s">
         <v>1122</v>
       </c>
       <c r="C65" s="59" t="s">
         <v>917</v>
       </c>
-      <c r="D65" s="71" t="s">
+      <c r="D65" s="70" t="s">
         <v>1039</v>
       </c>
       <c r="E65" s="60">
         <v>198</v>
       </c>
-      <c r="F65" s="71" t="s">
+      <c r="F65" s="70" t="s">
         <v>1038</v>
       </c>
-      <c r="G65" s="71" t="s">
+      <c r="G65" s="70" t="s">
         <v>1041</v>
       </c>
       <c r="H65" s="59" t="s">
@@ -8535,7 +8408,7 @@
       <c r="I65" s="59" t="s">
         <v>921</v>
       </c>
-      <c r="J65" s="70"/>
+      <c r="J65" s="69"/>
       <c r="K65" s="55" t="str">
         <f t="shared" si="0"/>
         <v>TC65_B25_offLabel_198_bizrul_True251unk_p</v>
@@ -8543,36 +8416,34 @@
       <c r="L65" s="55" t="s">
         <v>1211</v>
       </c>
-      <c r="M65" s="75" t="s">
+      <c r="M65" s="74" t="s">
         <v>1004</v>
       </c>
-      <c r="N65" s="75" t="s">
+      <c r="N65" s="74" t="s">
         <v>970</v>
       </c>
-      <c r="O65" s="72" t="s">
+      <c r="O65" s="71" t="s">
         <v>932</v>
       </c>
     </row>
     <row r="66" spans="1:15" ht="9.75" customHeight="1">
-      <c r="A66" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A66" s="54"/>
       <c r="B66" s="54" t="s">
         <v>1123</v>
       </c>
       <c r="C66" s="59" t="s">
         <v>917</v>
       </c>
-      <c r="D66" s="71" t="s">
+      <c r="D66" s="70" t="s">
         <v>1039</v>
       </c>
       <c r="E66" s="60">
         <v>198</v>
       </c>
-      <c r="F66" s="71" t="s">
+      <c r="F66" s="70" t="s">
         <v>1038</v>
       </c>
-      <c r="G66" s="71" t="s">
+      <c r="G66" s="70" t="s">
         <v>1042</v>
       </c>
       <c r="H66" s="59" t="s">
@@ -8581,7 +8452,7 @@
       <c r="I66" s="59" t="s">
         <v>925</v>
       </c>
-      <c r="J66" s="70"/>
+      <c r="J66" s="69"/>
       <c r="K66" s="55" t="str">
         <f t="shared" si="0"/>
         <v>TC66_B25_offLabel_198_bizrul_True251NA_p</v>
@@ -8589,36 +8460,34 @@
       <c r="L66" s="55" t="s">
         <v>1212</v>
       </c>
-      <c r="M66" s="75" t="s">
+      <c r="M66" s="74" t="s">
         <v>1005</v>
       </c>
-      <c r="N66" s="75" t="s">
+      <c r="N66" s="74" t="s">
         <v>971</v>
       </c>
-      <c r="O66" s="72" t="s">
+      <c r="O66" s="71" t="s">
         <v>934</v>
       </c>
     </row>
     <row r="67" spans="1:15" ht="9.75" customHeight="1">
-      <c r="A67" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A67" s="54"/>
       <c r="B67" s="54" t="s">
         <v>1124</v>
       </c>
       <c r="C67" s="59" t="s">
         <v>917</v>
       </c>
-      <c r="D67" s="71" t="s">
+      <c r="D67" s="70" t="s">
         <v>1039</v>
       </c>
       <c r="E67" s="60">
         <v>198</v>
       </c>
-      <c r="F67" s="71" t="s">
+      <c r="F67" s="70" t="s">
         <v>1038</v>
       </c>
-      <c r="G67" s="71" t="s">
+      <c r="G67" s="70" t="s">
         <v>1043</v>
       </c>
       <c r="H67" s="54" t="s">
@@ -8627,7 +8496,7 @@
       <c r="I67" s="59" t="s">
         <v>920</v>
       </c>
-      <c r="J67" s="70"/>
+      <c r="J67" s="69"/>
       <c r="K67" s="55" t="str">
         <f t="shared" ref="K67:K80" si="2">CONCATENATE(B67,"_",C67,"_",D67,"_",E67,"_",F67,"_",G67,"_",H67)</f>
         <v>TC67_B25_offLabel_198_bizrul_True251false_err</v>
@@ -8635,36 +8504,34 @@
       <c r="L67" s="55" t="s">
         <v>1213</v>
       </c>
-      <c r="M67" s="75" t="s">
+      <c r="M67" s="74" t="s">
         <v>1006</v>
       </c>
-      <c r="N67" s="75" t="s">
+      <c r="N67" s="74" t="s">
         <v>972</v>
       </c>
-      <c r="O67" s="73" t="s">
+      <c r="O67" s="72" t="s">
         <v>926</v>
       </c>
     </row>
     <row r="68" spans="1:15" ht="9.75" customHeight="1">
-      <c r="A68" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A68" s="54"/>
       <c r="B68" s="54" t="s">
         <v>1125</v>
       </c>
       <c r="C68" s="59" t="s">
         <v>917</v>
       </c>
-      <c r="D68" s="71" t="s">
+      <c r="D68" s="70" t="s">
         <v>1039</v>
       </c>
       <c r="E68" s="60">
         <v>198</v>
       </c>
-      <c r="F68" s="71" t="s">
+      <c r="F68" s="70" t="s">
         <v>1038</v>
       </c>
-      <c r="G68" s="71" t="s">
+      <c r="G68" s="70" t="s">
         <v>1044</v>
       </c>
       <c r="H68" s="54" t="s">
@@ -8673,7 +8540,7 @@
       <c r="I68" s="59" t="s">
         <v>930</v>
       </c>
-      <c r="J68" s="70"/>
+      <c r="J68" s="69"/>
       <c r="K68" s="55" t="str">
         <f t="shared" si="2"/>
         <v>TC68_B25_offLabel_198_bizrul_True251true_err</v>
@@ -8681,36 +8548,34 @@
       <c r="L68" s="55" t="s">
         <v>1214</v>
       </c>
-      <c r="M68" s="75" t="s">
+      <c r="M68" s="74" t="s">
         <v>1006</v>
       </c>
-      <c r="N68" s="75" t="s">
+      <c r="N68" s="74" t="s">
         <v>972</v>
       </c>
-      <c r="O68" s="73" t="s">
+      <c r="O68" s="72" t="s">
         <v>926</v>
       </c>
     </row>
     <row r="69" spans="1:15" ht="9.75" customHeight="1">
-      <c r="A69" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A69" s="54"/>
       <c r="B69" s="54" t="s">
         <v>1126</v>
       </c>
       <c r="C69" s="59" t="s">
         <v>917</v>
       </c>
-      <c r="D69" s="71" t="s">
+      <c r="D69" s="70" t="s">
         <v>1039</v>
       </c>
       <c r="E69" s="60">
         <v>197</v>
       </c>
-      <c r="F69" s="71" t="s">
+      <c r="F69" s="70" t="s">
         <v>1038</v>
       </c>
-      <c r="G69" s="71" t="s">
+      <c r="G69" s="70" t="s">
         <v>1045</v>
       </c>
       <c r="H69" s="59" t="s">
@@ -8719,7 +8584,7 @@
       <c r="I69" s="59" t="s">
         <v>922</v>
       </c>
-      <c r="J69" s="70"/>
+      <c r="J69" s="69"/>
       <c r="K69" s="55" t="str">
         <f t="shared" si="2"/>
         <v>TC69_B25_offLabel_197_bizrul_False251Null_p</v>
@@ -8727,36 +8592,34 @@
       <c r="L69" s="55" t="s">
         <v>1215</v>
       </c>
-      <c r="M69" s="75" t="s">
+      <c r="M69" s="74" t="s">
         <v>1007</v>
       </c>
-      <c r="N69" s="75" t="s">
+      <c r="N69" s="74" t="s">
         <v>973</v>
       </c>
-      <c r="O69" s="72" t="s">
+      <c r="O69" s="71" t="s">
         <v>933</v>
       </c>
     </row>
     <row r="70" spans="1:15" ht="9.75" customHeight="1">
-      <c r="A70" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A70" s="54"/>
       <c r="B70" s="54" t="s">
         <v>1127</v>
       </c>
       <c r="C70" s="59" t="s">
         <v>917</v>
       </c>
-      <c r="D70" s="71" t="s">
+      <c r="D70" s="70" t="s">
         <v>1039</v>
       </c>
       <c r="E70" s="60">
         <v>197</v>
       </c>
-      <c r="F70" s="71" t="s">
+      <c r="F70" s="70" t="s">
         <v>1038</v>
       </c>
-      <c r="G70" s="71" t="s">
+      <c r="G70" s="70" t="s">
         <v>1046</v>
       </c>
       <c r="H70" s="59" t="s">
@@ -8765,7 +8628,7 @@
       <c r="I70" s="59" t="s">
         <v>919</v>
       </c>
-      <c r="J70" s="70"/>
+      <c r="J70" s="69"/>
       <c r="K70" s="55" t="str">
         <f t="shared" si="2"/>
         <v>TC70_B25_offLabel_197_bizrul_False251true_p</v>
@@ -8773,36 +8636,34 @@
       <c r="L70" s="55" t="s">
         <v>1216</v>
       </c>
-      <c r="M70" s="75" t="s">
+      <c r="M70" s="74" t="s">
         <v>1008</v>
       </c>
-      <c r="N70" s="75" t="s">
+      <c r="N70" s="74" t="s">
         <v>974</v>
       </c>
-      <c r="O70" s="72" t="s">
+      <c r="O70" s="71" t="s">
         <v>928</v>
       </c>
     </row>
     <row r="71" spans="1:15" ht="9.75" customHeight="1">
-      <c r="A71" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A71" s="54"/>
       <c r="B71" s="54" t="s">
         <v>1128</v>
       </c>
       <c r="C71" s="59" t="s">
         <v>917</v>
       </c>
-      <c r="D71" s="71" t="s">
+      <c r="D71" s="70" t="s">
         <v>1039</v>
       </c>
       <c r="E71" s="60">
         <v>197</v>
       </c>
-      <c r="F71" s="71" t="s">
+      <c r="F71" s="70" t="s">
         <v>1038</v>
       </c>
-      <c r="G71" s="71" t="s">
+      <c r="G71" s="70" t="s">
         <v>1047</v>
       </c>
       <c r="H71" s="54" t="s">
@@ -8811,7 +8672,7 @@
       <c r="I71" s="59" t="s">
         <v>923</v>
       </c>
-      <c r="J71" s="70"/>
+      <c r="J71" s="69"/>
       <c r="K71" s="55" t="str">
         <f t="shared" si="2"/>
         <v>TC71_B25_offLabel_197_bizrul_False251false_err</v>
@@ -8819,36 +8680,34 @@
       <c r="L71" s="55" t="s">
         <v>1217</v>
       </c>
-      <c r="M71" s="75" t="s">
+      <c r="M71" s="74" t="s">
         <v>1009</v>
       </c>
-      <c r="N71" s="75" t="s">
+      <c r="N71" s="74" t="s">
         <v>975</v>
       </c>
-      <c r="O71" s="73" t="s">
+      <c r="O71" s="72" t="s">
         <v>927</v>
       </c>
     </row>
     <row r="72" spans="1:15" ht="9.75" customHeight="1">
-      <c r="A72" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A72" s="54"/>
       <c r="B72" s="54" t="s">
         <v>1129</v>
       </c>
       <c r="C72" s="59" t="s">
         <v>917</v>
       </c>
-      <c r="D72" s="71" t="s">
+      <c r="D72" s="70" t="s">
         <v>1039</v>
       </c>
       <c r="E72" s="60">
         <v>197</v>
       </c>
-      <c r="F72" s="71" t="s">
+      <c r="F72" s="70" t="s">
         <v>1038</v>
       </c>
-      <c r="G72" s="71" t="s">
+      <c r="G72" s="70" t="s">
         <v>1048</v>
       </c>
       <c r="H72" s="59" t="s">
@@ -8857,7 +8716,7 @@
       <c r="I72" s="59" t="s">
         <v>924</v>
       </c>
-      <c r="J72" s="70"/>
+      <c r="J72" s="69"/>
       <c r="K72" s="55" t="str">
         <f t="shared" si="2"/>
         <v>TC72_B25_offLabel_197_bizrul_false251unk_p</v>
@@ -8865,36 +8724,34 @@
       <c r="L72" s="55" t="s">
         <v>1218</v>
       </c>
-      <c r="M72" s="75" t="s">
+      <c r="M72" s="74" t="s">
         <v>1007</v>
       </c>
-      <c r="N72" s="75" t="s">
+      <c r="N72" s="74" t="s">
         <v>973</v>
       </c>
-      <c r="O72" s="72" t="s">
+      <c r="O72" s="71" t="s">
         <v>935</v>
       </c>
     </row>
     <row r="73" spans="1:15" ht="9.75" customHeight="1">
-      <c r="A73" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A73" s="54"/>
       <c r="B73" s="54" t="s">
         <v>1130</v>
       </c>
       <c r="C73" s="59" t="s">
         <v>917</v>
       </c>
-      <c r="D73" s="71" t="s">
+      <c r="D73" s="70" t="s">
         <v>1039</v>
       </c>
       <c r="E73" s="60">
         <v>197</v>
       </c>
-      <c r="F73" s="71" t="s">
+      <c r="F73" s="70" t="s">
         <v>1038</v>
       </c>
-      <c r="G73" s="71" t="s">
+      <c r="G73" s="70" t="s">
         <v>1049</v>
       </c>
       <c r="H73" s="59" t="s">
@@ -8903,7 +8760,7 @@
       <c r="I73" s="59" t="s">
         <v>929</v>
       </c>
-      <c r="J73" s="70"/>
+      <c r="J73" s="69"/>
       <c r="K73" s="55" t="str">
         <f t="shared" si="2"/>
         <v>TC73_B25_offLabel_197_bizrul_false251NA_p</v>
@@ -8911,42 +8768,40 @@
       <c r="L73" s="55" t="s">
         <v>1219</v>
       </c>
-      <c r="M73" s="75" t="s">
+      <c r="M73" s="74" t="s">
         <v>1007</v>
       </c>
-      <c r="N73" s="75" t="s">
+      <c r="N73" s="74" t="s">
         <v>973</v>
       </c>
-      <c r="O73" s="72" t="s">
+      <c r="O73" s="71" t="s">
         <v>936</v>
       </c>
     </row>
     <row r="74" spans="1:15" ht="9.75" customHeight="1">
-      <c r="A74" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A74" s="54"/>
       <c r="B74" s="54" t="s">
         <v>1131</v>
       </c>
       <c r="C74" s="59" t="s">
         <v>917</v>
       </c>
-      <c r="D74" s="71" t="s">
+      <c r="D74" s="70" t="s">
         <v>1039</v>
       </c>
       <c r="E74" s="60">
         <v>197</v>
       </c>
-      <c r="F74" s="71" t="s">
+      <c r="F74" s="70" t="s">
         <v>1038</v>
       </c>
-      <c r="G74" s="71" t="s">
+      <c r="G74" s="70" t="s">
         <v>1050</v>
       </c>
       <c r="H74" s="54" t="s">
         <v>1142</v>
       </c>
-      <c r="I74" s="71" t="s">
+      <c r="I74" s="70" t="s">
         <v>938</v>
       </c>
       <c r="K74" s="55" t="str">
@@ -8956,42 +8811,40 @@
       <c r="L74" s="55" t="s">
         <v>1220</v>
       </c>
-      <c r="M74" s="75" t="s">
+      <c r="M74" s="74" t="s">
         <v>1010</v>
       </c>
-      <c r="N74" s="75" t="s">
+      <c r="N74" s="74" t="s">
         <v>976</v>
       </c>
-      <c r="O74" s="73" t="s">
+      <c r="O74" s="72" t="s">
         <v>937</v>
       </c>
     </row>
     <row r="75" spans="1:15" ht="9.75" customHeight="1">
-      <c r="A75" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A75" s="54"/>
       <c r="B75" s="54" t="s">
         <v>1132</v>
       </c>
       <c r="C75" s="59" t="s">
         <v>917</v>
       </c>
-      <c r="D75" s="71" t="s">
+      <c r="D75" s="70" t="s">
         <v>1039</v>
       </c>
       <c r="E75" s="60">
         <v>197</v>
       </c>
-      <c r="F75" s="71" t="s">
+      <c r="F75" s="70" t="s">
         <v>1038</v>
       </c>
-      <c r="G75" s="71" t="s">
+      <c r="G75" s="70" t="s">
         <v>1051</v>
       </c>
       <c r="H75" s="54" t="s">
         <v>1142</v>
       </c>
-      <c r="I75" s="71" t="s">
+      <c r="I75" s="70" t="s">
         <v>940</v>
       </c>
       <c r="K75" s="55" t="str">
@@ -9001,42 +8854,40 @@
       <c r="L75" s="55" t="s">
         <v>1221</v>
       </c>
-      <c r="M75" s="75" t="s">
+      <c r="M75" s="74" t="s">
         <v>1010</v>
       </c>
-      <c r="N75" s="75" t="s">
+      <c r="N75" s="74" t="s">
         <v>976</v>
       </c>
-      <c r="O75" s="73" t="s">
+      <c r="O75" s="72" t="s">
         <v>937</v>
       </c>
     </row>
     <row r="76" spans="1:15" ht="9.75" customHeight="1">
-      <c r="A76" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A76" s="54"/>
       <c r="B76" s="54" t="s">
         <v>1133</v>
       </c>
       <c r="C76" s="59" t="s">
         <v>917</v>
       </c>
-      <c r="D76" s="71" t="s">
+      <c r="D76" s="70" t="s">
         <v>1039</v>
       </c>
       <c r="E76" s="60">
         <v>197</v>
       </c>
-      <c r="F76" s="71" t="s">
+      <c r="F76" s="70" t="s">
         <v>1038</v>
       </c>
-      <c r="G76" s="71" t="s">
+      <c r="G76" s="70" t="s">
         <v>1052</v>
       </c>
       <c r="H76" s="54" t="s">
         <v>1142</v>
       </c>
-      <c r="I76" s="71" t="s">
+      <c r="I76" s="70" t="s">
         <v>941</v>
       </c>
       <c r="K76" s="55" t="str">
@@ -9046,42 +8897,40 @@
       <c r="L76" s="55" t="s">
         <v>1222</v>
       </c>
-      <c r="M76" s="75" t="s">
+      <c r="M76" s="74" t="s">
         <v>1011</v>
       </c>
-      <c r="N76" s="75" t="s">
+      <c r="N76" s="74" t="s">
         <v>977</v>
       </c>
-      <c r="O76" s="73" t="s">
+      <c r="O76" s="72" t="s">
         <v>939</v>
       </c>
     </row>
     <row r="77" spans="1:15" ht="9.75" customHeight="1">
-      <c r="A77" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A77" s="54"/>
       <c r="B77" s="54" t="s">
         <v>1134</v>
       </c>
       <c r="C77" s="59" t="s">
         <v>917</v>
       </c>
-      <c r="D77" s="71" t="s">
+      <c r="D77" s="70" t="s">
         <v>1039</v>
       </c>
       <c r="E77" s="60">
         <v>197</v>
       </c>
-      <c r="F77" s="71" t="s">
+      <c r="F77" s="70" t="s">
         <v>1038</v>
       </c>
-      <c r="G77" s="71" t="s">
+      <c r="G77" s="70" t="s">
         <v>1053</v>
       </c>
       <c r="H77" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="I77" s="71" t="s">
+      <c r="I77" s="70" t="s">
         <v>941</v>
       </c>
       <c r="K77" s="55" t="str">
@@ -9091,38 +8940,36 @@
       <c r="L77" s="55" t="s">
         <v>1223</v>
       </c>
-      <c r="M77" s="75"/>
-      <c r="N77" s="75"/>
-      <c r="O77" s="72" t="s">
+      <c r="M77" s="74"/>
+      <c r="N77" s="74"/>
+      <c r="O77" s="71" t="s">
         <v>942</v>
       </c>
     </row>
     <row r="78" spans="1:15" ht="9.75" customHeight="1">
-      <c r="A78" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A78" s="54"/>
       <c r="B78" s="54" t="s">
         <v>1135</v>
       </c>
       <c r="C78" s="59" t="s">
         <v>917</v>
       </c>
-      <c r="D78" s="71" t="s">
+      <c r="D78" s="70" t="s">
         <v>1039</v>
       </c>
       <c r="E78" s="60">
         <v>197</v>
       </c>
-      <c r="F78" s="71" t="s">
+      <c r="F78" s="70" t="s">
         <v>1038</v>
       </c>
-      <c r="G78" s="71" t="s">
+      <c r="G78" s="70" t="s">
         <v>1054</v>
       </c>
       <c r="H78" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="I78" s="71" t="s">
+      <c r="I78" s="70" t="s">
         <v>944</v>
       </c>
       <c r="K78" s="55" t="str">
@@ -9132,38 +8979,36 @@
       <c r="L78" s="55" t="s">
         <v>1224</v>
       </c>
-      <c r="M78" s="75"/>
-      <c r="N78" s="75"/>
-      <c r="O78" s="72" t="s">
+      <c r="M78" s="74"/>
+      <c r="N78" s="74"/>
+      <c r="O78" s="71" t="s">
         <v>943</v>
       </c>
     </row>
     <row r="79" spans="1:15" ht="9.75" customHeight="1">
-      <c r="A79" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A79" s="54"/>
       <c r="B79" s="54" t="s">
         <v>1136</v>
       </c>
       <c r="C79" s="59" t="s">
         <v>917</v>
       </c>
-      <c r="D79" s="71" t="s">
+      <c r="D79" s="70" t="s">
         <v>1039</v>
       </c>
       <c r="E79" s="60">
         <v>197</v>
       </c>
-      <c r="F79" s="71" t="s">
+      <c r="F79" s="70" t="s">
         <v>1038</v>
       </c>
-      <c r="G79" s="71" t="s">
+      <c r="G79" s="70" t="s">
         <v>1055</v>
       </c>
       <c r="H79" s="54" t="s">
         <v>1142</v>
       </c>
-      <c r="I79" s="71" t="s">
+      <c r="I79" s="70" t="s">
         <v>944</v>
       </c>
       <c r="K79" s="55" t="str">
@@ -9173,42 +9018,40 @@
       <c r="L79" s="55" t="s">
         <v>1225</v>
       </c>
-      <c r="M79" s="75" t="s">
+      <c r="M79" s="74" t="s">
         <v>1009</v>
       </c>
-      <c r="N79" s="75" t="s">
+      <c r="N79" s="74" t="s">
         <v>975</v>
       </c>
-      <c r="O79" s="73" t="s">
+      <c r="O79" s="72" t="s">
         <v>927</v>
       </c>
     </row>
     <row r="80" spans="1:15" ht="9.75" customHeight="1">
-      <c r="A80" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="A80" s="54"/>
       <c r="B80" s="54" t="s">
         <v>1137</v>
       </c>
       <c r="C80" s="59" t="s">
         <v>917</v>
       </c>
-      <c r="D80" s="71" t="s">
+      <c r="D80" s="70" t="s">
         <v>1039</v>
       </c>
       <c r="E80" s="60">
         <v>197</v>
       </c>
-      <c r="F80" s="71" t="s">
+      <c r="F80" s="70" t="s">
         <v>1038</v>
       </c>
-      <c r="G80" s="71" t="s">
+      <c r="G80" s="70" t="s">
         <v>1056</v>
       </c>
       <c r="H80" s="54" t="s">
         <v>1142</v>
       </c>
-      <c r="I80" s="71" t="s">
+      <c r="I80" s="70" t="s">
         <v>945</v>
       </c>
       <c r="K80" s="55" t="str">
@@ -9218,13 +9061,13 @@
       <c r="L80" s="55" t="s">
         <v>1226</v>
       </c>
-      <c r="M80" s="75" t="s">
+      <c r="M80" s="74" t="s">
         <v>1010</v>
       </c>
-      <c r="N80" s="75" t="s">
+      <c r="N80" s="74" t="s">
         <v>976</v>
       </c>
-      <c r="O80" s="73" t="s">
+      <c r="O80" s="72" t="s">
         <v>937</v>
       </c>
     </row>

</xml_diff>